<commit_message>
The original service list I made before you guys went to RappK and some attempted decennial and migration stuff. Might still be of use -Mousa
</commit_message>
<xml_diff>
--- a/Services.xlsx
+++ b/Services.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mousa The 14\Documents\DSPG2021\RAPPK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0208A102-939B-49C0-9CD9-FC2C513C2A06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE325DB6-20B1-47E3-B4A7-84B24C982F26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{6D336315-7F54-40BE-916C-D16286ADC43E}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6D336315-7F54-40BE-916C-D16286ADC43E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -542,7 +542,7 @@
   <dimension ref="B2:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>